<commit_message>
Proyecto De Pagina Final
</commit_message>
<xml_diff>
--- a/Proyrcto de pagina/ADSO00nEV01nLCHnActividadnhtml___1464147c84746db___ (1).xlsx
+++ b/Proyrcto de pagina/ADSO00nEV01nLCHnActividadnhtml___1464147c84746db___ (1).xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10313"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sena/Desktop/cml/trabajo instructor/Sena/Formación/2023/ADSO 2699192/Actividad-html/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jaive\OneDrive\Escritorio\Proyrcto de pagina\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C274B601-6C0B-FF45-9EFA-DD4D9A2ACF7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11433A08-84E6-40E0-97E4-097DE877EC64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="23040" windowHeight="13000" xr2:uid="{AF3AE176-B3AF-4D49-B778-54BC367B98FB}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{AF3AE176-B3AF-4D49-B778-54BC367B98FB}"/>
   </bookViews>
   <sheets>
     <sheet name="Formato lista chequeo" sheetId="5" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191028"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -23,9 +23,12 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -106,14 +109,14 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
   <futureMetadata name="XLDAPR" count="1">
     <bk>
       <extLst>
-        <ext xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray" uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
           <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
         </ext>
       </extLst>
@@ -333,11 +336,11 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="9" fontId="4" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -345,20 +348,6 @@
     <cellStyle name="Porcentaje" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="6">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -374,6 +363,20 @@
     <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -394,12 +397,12 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{471DF5DC-2D96-4118-87A8-A1F84D8A0B5E}" name="Chequeo_Portafolio" displayName="Chequeo_Portafolio" ref="A12:E27" totalsRowShown="0" headerRowDxfId="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{471DF5DC-2D96-4118-87A8-A1F84D8A0B5E}" name="Chequeo_Portafolio" displayName="Chequeo_Portafolio" ref="A12:E27" totalsRowShown="0" headerRowDxfId="3">
   <autoFilter ref="A12:E27" xr:uid="{0DBC0078-45CE-4122-B256-DBD33A3CD2F1}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{11B3BFEC-F814-485F-8954-195DAED203C9}" name="ID CRITERIO" dataDxfId="4"/>
-    <tableColumn id="2" xr3:uid="{8000FBBA-787F-458A-9EA4-C8B2CA56425C}" name="CRITERIO" dataDxfId="3"/>
-    <tableColumn id="3" xr3:uid="{0F6CF467-B2D1-4121-8E1D-9FF7609D6DF4}" name="CALIFICACION" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{11B3BFEC-F814-485F-8954-195DAED203C9}" name="ID CRITERIO" dataDxfId="2"/>
+    <tableColumn id="2" xr3:uid="{8000FBBA-787F-458A-9EA4-C8B2CA56425C}" name="CRITERIO" dataDxfId="1"/>
+    <tableColumn id="3" xr3:uid="{0F6CF467-B2D1-4121-8E1D-9FF7609D6DF4}" name="CALIFICACION" dataDxfId="0"/>
     <tableColumn id="4" xr3:uid="{D319A72D-18D1-417E-B675-4A9E51062384}" name="OBSERVACION"/>
     <tableColumn id="5" xr3:uid="{6F3F9C5B-7F28-416B-8E8A-F9E103D7D118}" name="PUNTAJE">
       <calculatedColumnFormula>100/15*Chequeo_Portafolio[[#This Row],[CALIFICACION]]</calculatedColumnFormula>
@@ -717,20 +720,20 @@
   <dimension ref="A2:E27"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="12" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B26" sqref="B26"/>
+      <pane ySplit="12" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.1640625" customWidth="1"/>
-    <col min="2" max="2" width="73.6640625" customWidth="1"/>
-    <col min="3" max="3" width="16.5" customWidth="1"/>
+    <col min="1" max="1" width="14.140625" customWidth="1"/>
+    <col min="2" max="2" width="73.7109375" customWidth="1"/>
+    <col min="3" max="3" width="16.42578125" customWidth="1"/>
     <col min="4" max="4" width="19" customWidth="1"/>
-    <col min="5" max="5" width="12.6640625" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="12.7109375" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -738,7 +741,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
@@ -746,19 +749,19 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B4" s="3"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B5" s="3"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>4</v>
       </c>
@@ -766,34 +769,34 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B7" s="4" t="str">
         <f>IF(A10&gt;=0.9,"APROBADO","NO APROBADO")</f>
-        <v>NO APROBADO</v>
+        <v>APROBADO</v>
       </c>
       <c r="D7" s="9"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B8" s="8"/>
       <c r="D8" s="9"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B9" s="8"/>
       <c r="D9" s="9"/>
     </row>
-    <row r="10" spans="1:5" ht="24" x14ac:dyDescent="0.3">
-      <c r="A10" s="11" cm="1">
+    <row r="10" spans="1:5" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A10" s="12" cm="1">
         <f t="array" ref="A10">SUM(Chequeo_Portafolio[PUNTAJE]/100)</f>
-        <v>0</v>
-      </c>
-      <c r="B10" s="11"/>
-      <c r="C10" s="11"/>
-      <c r="D10" s="11"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+        <v>0.93333333333333324</v>
+      </c>
+      <c r="B10" s="12"/>
+      <c r="C10" s="12"/>
+      <c r="D10" s="12"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>6</v>
       </c>
@@ -810,7 +813,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>1</v>
       </c>
@@ -818,14 +821,14 @@
         <v>26</v>
       </c>
       <c r="C13" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E13">
         <f>100/15*Chequeo_Portafolio[[#This Row],[CALIFICACION]]</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+        <v>6.666666666666667</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>2</v>
       </c>
@@ -833,14 +836,14 @@
         <v>18</v>
       </c>
       <c r="C14" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E14">
         <f>100/15*Chequeo_Portafolio[[#This Row],[CALIFICACION]]</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+        <v>6.666666666666667</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>3</v>
       </c>
@@ -848,14 +851,14 @@
         <v>22</v>
       </c>
       <c r="C15" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E15">
         <f>100/15*Chequeo_Portafolio[[#This Row],[CALIFICACION]]</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+        <v>6.666666666666667</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>4</v>
       </c>
@@ -863,14 +866,14 @@
         <v>17</v>
       </c>
       <c r="C16" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E16">
         <f>100/15*Chequeo_Portafolio[[#This Row],[CALIFICACION]]</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+        <v>6.666666666666667</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>5</v>
       </c>
@@ -878,14 +881,14 @@
         <v>14</v>
       </c>
       <c r="C17" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E17">
         <f>100/15*Chequeo_Portafolio[[#This Row],[CALIFICACION]]</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+        <v>6.666666666666667</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>6</v>
       </c>
@@ -893,14 +896,14 @@
         <v>15</v>
       </c>
       <c r="C18" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E18">
         <f>100/15*Chequeo_Portafolio[[#This Row],[CALIFICACION]]</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+        <v>6.666666666666667</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>7</v>
       </c>
@@ -908,14 +911,14 @@
         <v>16</v>
       </c>
       <c r="C19" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E19">
         <f>100/15*Chequeo_Portafolio[[#This Row],[CALIFICACION]]</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+        <v>6.666666666666667</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>8</v>
       </c>
@@ -923,14 +926,14 @@
         <v>21</v>
       </c>
       <c r="C20" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E20">
         <f>100/15*Chequeo_Portafolio[[#This Row],[CALIFICACION]]</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+        <v>6.666666666666667</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>9</v>
       </c>
@@ -938,14 +941,14 @@
         <v>20</v>
       </c>
       <c r="C21" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E21">
         <f>100/15*Chequeo_Portafolio[[#This Row],[CALIFICACION]]</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+        <v>6.666666666666667</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>10</v>
       </c>
@@ -953,14 +956,14 @@
         <v>19</v>
       </c>
       <c r="C22" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E22">
         <f>100/15*Chequeo_Portafolio[[#This Row],[CALIFICACION]]</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+        <v>6.666666666666667</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>11</v>
       </c>
@@ -968,14 +971,14 @@
         <v>23</v>
       </c>
       <c r="C23" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E23">
         <f>100/15*Chequeo_Portafolio[[#This Row],[CALIFICACION]]</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+        <v>6.666666666666667</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>12</v>
       </c>
@@ -983,14 +986,14 @@
         <v>24</v>
       </c>
       <c r="C24" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E24">
         <f>100/15*Chequeo_Portafolio[[#This Row],[CALIFICACION]]</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+        <v>6.666666666666667</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>13</v>
       </c>
@@ -998,18 +1001,18 @@
         <v>27</v>
       </c>
       <c r="C25" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E25">
         <f>100/15*Chequeo_Portafolio[[#This Row],[CALIFICACION]]</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+        <v>6.666666666666667</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>14</v>
       </c>
-      <c r="B26" s="12"/>
+      <c r="B26" s="11"/>
       <c r="C26" s="1">
         <v>0</v>
       </c>
@@ -1018,19 +1021,19 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:5" ht="48" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>15</v>
       </c>
-      <c r="B27" s="12" t="s">
+      <c r="B27" s="11" t="s">
         <v>25</v>
       </c>
       <c r="C27" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E27">
         <f>100/15*Chequeo_Portafolio[[#This Row],[CALIFICACION]]</f>
-        <v>0</v>
+        <v>6.666666666666667</v>
       </c>
     </row>
   </sheetData>
@@ -1053,10 +1056,10 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B7">
-    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="NO APROBADO">
+    <cfRule type="containsText" dxfId="5" priority="2" operator="containsText" text="NO APROBADO">
       <formula>NOT(ISERROR(SEARCH("NO APROBADO",B7)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="0" priority="3" operator="containsText" text="APROBADO">
+    <cfRule type="containsText" dxfId="4" priority="3" operator="containsText" text="APROBADO">
       <formula>NOT(ISERROR(SEARCH("APROBADO",B7)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1108,6 +1111,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100E9065DAD1227714FA979735511B50406" ma:contentTypeVersion="0" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="7cc61fc4a835c57ebc89b58c5b4789d3">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="5b2b1fa7a59e354d7f595b7732424404">
     <xsd:element name="properties">
@@ -1221,22 +1239,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{53E77349-AD5A-4890-A8E0-61A1A5FF3E5A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{58204219-3B34-460D-8848-4415374C54F6}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F89442E1-F58A-4A63-9B2A-7534D891220B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1250,21 +1270,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{58204219-3B34-460D-8848-4415374C54F6}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{53E77349-AD5A-4890-A8E0-61A1A5FF3E5A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>